<commit_message>
Deploying to gh-pages from  @ 996afe27891c487d80ff6172610c53e4c7956804 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/3.a.1.xlsx
+++ b/en/downloads/data-excel/3.a.1.xlsx
@@ -486,7 +486,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -568,7 +568,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -600,6 +599,15 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -909,7 +917,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -965,6 +975,9 @@
       <c r="F4" s="8">
         <v>2020</v>
       </c>
+      <c r="G4" s="8">
+        <v>2021</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
@@ -976,14 +989,17 @@
       <c r="C5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="38">
+      <c r="D5" s="37">
         <v>8.3000000000000007</v>
       </c>
-      <c r="E5" s="38">
+      <c r="E5" s="37">
         <v>8.1</v>
       </c>
-      <c r="F5" s="38">
+      <c r="F5" s="37">
         <v>7.6</v>
+      </c>
+      <c r="G5" s="40">
+        <v>6.3</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -996,9 +1012,10 @@
       <c r="C6" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="40"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
@@ -1010,14 +1027,17 @@
       <c r="C7" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="39">
+      <c r="D7" s="38">
         <v>17.7</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="38">
         <v>17.2</v>
       </c>
-      <c r="F7" s="39">
+      <c r="F7" s="38">
         <v>16</v>
+      </c>
+      <c r="G7" s="41">
+        <v>13.4</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1030,14 +1050,17 @@
       <c r="C8" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="39">
+      <c r="D8" s="38">
         <v>0.5</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="38">
         <v>0.4</v>
       </c>
-      <c r="F8" s="39">
+      <c r="F8" s="38">
         <v>0.5</v>
+      </c>
+      <c r="G8" s="41">
+        <v>0.4</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1050,9 +1073,10 @@
       <c r="C9" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="41"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
@@ -1064,14 +1088,17 @@
       <c r="C10" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="39">
+      <c r="D10" s="38">
         <v>6.4</v>
       </c>
-      <c r="E10" s="39">
+      <c r="E10" s="38">
         <v>6.2</v>
       </c>
-      <c r="F10" s="39">
+      <c r="F10" s="38">
         <v>6.2</v>
+      </c>
+      <c r="G10" s="41">
+        <v>5.3</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1084,14 +1111,17 @@
       <c r="C11" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="39">
+      <c r="D11" s="38">
         <v>9.5</v>
       </c>
-      <c r="E11" s="39">
+      <c r="E11" s="38">
         <v>9.1999999999999993</v>
       </c>
-      <c r="F11" s="39">
+      <c r="F11" s="38">
         <v>8.5</v>
+      </c>
+      <c r="G11" s="41">
+        <v>6.9</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1104,9 +1134,10 @@
       <c r="C12" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="41"/>
     </row>
     <row r="13" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
@@ -1118,14 +1149,17 @@
       <c r="C13" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="39">
+      <c r="D13" s="38">
         <v>10.8</v>
       </c>
-      <c r="E13" s="39">
+      <c r="E13" s="38">
         <v>10.9</v>
       </c>
-      <c r="F13" s="39">
+      <c r="F13" s="38">
         <v>9.8000000000000007</v>
+      </c>
+      <c r="G13" s="41">
+        <v>9.1</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -1138,14 +1172,17 @@
       <c r="C14" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="39">
+      <c r="D14" s="38">
         <v>3.4</v>
       </c>
-      <c r="E14" s="39">
+      <c r="E14" s="38">
         <v>4.4000000000000004</v>
       </c>
-      <c r="F14" s="39">
+      <c r="F14" s="38">
         <v>2.8</v>
+      </c>
+      <c r="G14" s="41">
+        <v>1.9</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -1158,16 +1195,18 @@
       <c r="C15" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="39">
+      <c r="D15" s="38">
         <v>17.899999999999999</v>
       </c>
-      <c r="E15" s="39">
+      <c r="E15" s="38">
         <v>17</v>
       </c>
-      <c r="F15" s="39">
+      <c r="F15" s="38">
         <v>15.7</v>
       </c>
-      <c r="G15" s="29"/>
+      <c r="G15" s="41">
+        <v>15.2</v>
+      </c>
     </row>
     <row r="16" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
@@ -1179,14 +1218,17 @@
       <c r="C16" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="39">
+      <c r="D16" s="38">
         <v>14.7</v>
       </c>
-      <c r="E16" s="39">
+      <c r="E16" s="38">
         <v>13.8</v>
       </c>
-      <c r="F16" s="39">
+      <c r="F16" s="38">
         <v>14.2</v>
+      </c>
+      <c r="G16" s="41">
+        <v>12.7</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -1199,14 +1241,17 @@
       <c r="C17" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="39">
+      <c r="D17" s="38">
         <v>6.7</v>
       </c>
-      <c r="E17" s="39">
+      <c r="E17" s="38">
         <v>6</v>
       </c>
-      <c r="F17" s="39">
+      <c r="F17" s="38">
         <v>6.2</v>
+      </c>
+      <c r="G17" s="41">
+        <v>4.3</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -1219,14 +1264,17 @@
       <c r="C18" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="39">
+      <c r="D18" s="38">
         <v>13</v>
       </c>
-      <c r="E18" s="39">
+      <c r="E18" s="38">
         <v>13.7</v>
       </c>
-      <c r="F18" s="39">
+      <c r="F18" s="38">
         <v>13.5</v>
+      </c>
+      <c r="G18" s="41">
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -1239,14 +1287,17 @@
       <c r="C19" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="39">
+      <c r="D19" s="38">
         <v>12.2</v>
       </c>
-      <c r="E19" s="39">
+      <c r="E19" s="38">
         <v>10.5</v>
       </c>
-      <c r="F19" s="39">
+      <c r="F19" s="38">
         <v>9.4</v>
+      </c>
+      <c r="G19" s="41">
+        <v>7.8</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -1259,16 +1310,18 @@
       <c r="C20" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="39">
+      <c r="D20" s="38">
         <v>6.2</v>
       </c>
-      <c r="E20" s="39">
+      <c r="E20" s="38">
         <v>6.3</v>
       </c>
-      <c r="F20" s="39">
+      <c r="F20" s="38">
         <v>7.3</v>
       </c>
-      <c r="G20" s="29"/>
+      <c r="G20" s="41">
+        <v>5.5</v>
+      </c>
     </row>
     <row r="21" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
@@ -1280,14 +1333,17 @@
       <c r="C21" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="39">
+      <c r="D21" s="38">
         <v>1.8</v>
       </c>
-      <c r="E21" s="39">
+      <c r="E21" s="38">
         <v>1.6</v>
       </c>
-      <c r="F21" s="39">
+      <c r="F21" s="38">
         <v>1.3</v>
+      </c>
+      <c r="G21" s="41">
+        <v>1.2</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -1300,10 +1356,10 @@
       <c r="C22" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="18"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="41"/>
     </row>
     <row r="23" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
@@ -1315,16 +1371,18 @@
       <c r="C23" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="D23" s="39">
+      <c r="D23" s="38">
         <v>0.4</v>
       </c>
-      <c r="E23" s="39">
+      <c r="E23" s="38">
         <v>0.3</v>
       </c>
-      <c r="F23" s="39">
+      <c r="F23" s="38">
         <v>0.4</v>
       </c>
-      <c r="G23" s="18"/>
+      <c r="G23" s="41">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="24" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
@@ -1336,16 +1394,18 @@
       <c r="C24" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="D24" s="39">
+      <c r="D24" s="38">
         <v>10.6</v>
       </c>
-      <c r="E24" s="39">
+      <c r="E24" s="38">
         <v>10</v>
       </c>
-      <c r="F24" s="39">
+      <c r="F24" s="38">
         <v>9.4</v>
       </c>
-      <c r="G24" s="18"/>
+      <c r="G24" s="41">
+        <v>7.4</v>
+      </c>
     </row>
     <row r="25" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
@@ -1357,256 +1417,278 @@
       <c r="C25" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="D25" s="39">
+      <c r="D25" s="38">
         <v>10</v>
       </c>
-      <c r="E25" s="39">
+      <c r="E25" s="38">
         <v>10.199999999999999</v>
       </c>
-      <c r="F25" s="39">
+      <c r="F25" s="38">
         <v>9.4</v>
       </c>
-      <c r="G25" s="18"/>
+      <c r="G25" s="41">
+        <v>9</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="C26" s="31" t="s">
+      <c r="C26" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="18"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="41"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="32" t="s">
+      <c r="A27" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="B27" s="33" t="s">
+      <c r="B27" s="32" t="s">
         <v>86</v>
       </c>
       <c r="C27" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="D27" s="39">
+      <c r="D27" s="38">
         <v>2.8</v>
       </c>
-      <c r="E27" s="39">
+      <c r="E27" s="38">
         <v>3.4</v>
       </c>
-      <c r="F27" s="39">
+      <c r="F27" s="38">
         <v>2.8</v>
       </c>
-      <c r="G27" s="18"/>
+      <c r="G27" s="41">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="33" t="s">
+      <c r="B28" s="32" t="s">
         <v>55</v>
       </c>
       <c r="C28" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="D28" s="39">
+      <c r="D28" s="38">
         <v>3.5</v>
       </c>
-      <c r="E28" s="39">
+      <c r="E28" s="38">
         <v>2.9</v>
       </c>
-      <c r="F28" s="39">
+      <c r="F28" s="38">
         <v>3.8</v>
       </c>
-      <c r="G28" s="18"/>
+      <c r="G28" s="41">
+        <v>2.9</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="33" t="s">
+      <c r="B29" s="32" t="s">
         <v>57</v>
       </c>
       <c r="C29" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="D29" s="39">
+      <c r="D29" s="38">
         <v>9.8000000000000007</v>
       </c>
-      <c r="E29" s="39">
+      <c r="E29" s="38">
         <v>9.3000000000000007</v>
       </c>
-      <c r="F29" s="39">
+      <c r="F29" s="38">
         <v>8.8000000000000007</v>
       </c>
-      <c r="G29" s="18"/>
+      <c r="G29" s="41">
+        <v>7.4</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="32" t="s">
+      <c r="A30" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="33" t="s">
+      <c r="B30" s="32" t="s">
         <v>59</v>
       </c>
       <c r="C30" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="D30" s="39">
+      <c r="D30" s="38">
         <v>11.7</v>
       </c>
-      <c r="E30" s="39">
+      <c r="E30" s="38">
         <v>11.8</v>
       </c>
-      <c r="F30" s="39">
+      <c r="F30" s="38">
         <v>10.8</v>
       </c>
-      <c r="G30" s="18"/>
+      <c r="G30" s="41">
+        <v>9.1</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="32" t="s">
+      <c r="A31" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="33" t="s">
+      <c r="B31" s="32" t="s">
         <v>61</v>
       </c>
       <c r="C31" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="D31" s="39">
+      <c r="D31" s="38">
         <v>5.6</v>
       </c>
-      <c r="E31" s="39">
+      <c r="E31" s="38">
         <v>5.5</v>
       </c>
-      <c r="F31" s="39">
+      <c r="F31" s="38">
         <v>4.9000000000000004</v>
       </c>
-      <c r="G31" s="18"/>
+      <c r="G31" s="41">
+        <v>4.0999999999999996</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="30" t="s">
+      <c r="B32" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="C32" s="31" t="s">
+      <c r="C32" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="D32" s="39"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="18"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="41"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="34" t="s">
+      <c r="A33" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="B33" s="33" t="s">
+      <c r="B33" s="32" t="s">
         <v>65</v>
       </c>
       <c r="C33" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D33" s="39">
+      <c r="D33" s="38">
         <v>8</v>
       </c>
-      <c r="E33" s="39">
+      <c r="E33" s="38">
         <v>8.1999999999999993</v>
       </c>
-      <c r="F33" s="39">
+      <c r="F33" s="38">
         <v>7.9</v>
       </c>
-      <c r="G33" s="18"/>
+      <c r="G33" s="41">
+        <v>6.4</v>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="34" t="s">
+      <c r="A34" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="33" t="s">
+      <c r="B34" s="32" t="s">
         <v>67</v>
       </c>
       <c r="C34" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="D34" s="39">
+      <c r="D34" s="38">
         <v>7.4</v>
       </c>
-      <c r="E34" s="39">
+      <c r="E34" s="38">
         <v>7.8</v>
       </c>
-      <c r="F34" s="39">
+      <c r="F34" s="38">
         <v>6.9</v>
       </c>
-      <c r="G34" s="18"/>
+      <c r="G34" s="41">
+        <v>6.2</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="34" t="s">
+      <c r="A35" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="33" t="s">
+      <c r="B35" s="32" t="s">
         <v>69</v>
       </c>
       <c r="C35" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="D35" s="39">
+      <c r="D35" s="38">
         <v>8.5</v>
       </c>
-      <c r="E35" s="39">
+      <c r="E35" s="38">
         <v>7.7</v>
       </c>
-      <c r="F35" s="39">
+      <c r="F35" s="38">
         <v>8</v>
       </c>
-      <c r="G35" s="18"/>
+      <c r="G35" s="41">
+        <v>5.4</v>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="B36" s="33" t="s">
+      <c r="B36" s="32" t="s">
         <v>71</v>
       </c>
       <c r="C36" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="D36" s="39">
+      <c r="D36" s="38">
         <v>8.5</v>
       </c>
-      <c r="E36" s="39">
+      <c r="E36" s="38">
         <v>8</v>
       </c>
-      <c r="F36" s="39">
+      <c r="F36" s="38">
         <v>7.2</v>
       </c>
-      <c r="G36" s="18"/>
+      <c r="G36" s="41">
+        <v>6.6</v>
+      </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="35" t="s">
+      <c r="A37" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="36" t="s">
+      <c r="B37" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="C37" s="37" t="s">
+      <c r="C37" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="D37" s="40">
+      <c r="D37" s="39">
         <v>9.6</v>
       </c>
-      <c r="E37" s="40">
+      <c r="E37" s="39">
         <v>8.8000000000000007</v>
       </c>
-      <c r="F37" s="40">
+      <c r="F37" s="39">
         <v>8.1</v>
       </c>
-      <c r="G37" s="18"/>
+      <c r="G37" s="42">
+        <v>7.2</v>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D38" s="18"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ e495a6ad9f9dfed8f9d72973afec93deac66d484 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/3.a.1.xlsx
+++ b/en/downloads/data-excel/3.a.1.xlsx
@@ -329,7 +329,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -431,6 +431,12 @@
       <family val="1"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Times New Roman Cyr"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -486,7 +492,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -608,6 +614,13 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -915,10 +928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -929,7 +942,7 @@
     <col min="4" max="6" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>101</v>
       </c>
@@ -944,7 +957,7 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -955,8 +968,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -978,8 +991,11 @@
       <c r="G4" s="8">
         <v>2021</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="8">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>6</v>
       </c>
@@ -1001,8 +1017,11 @@
       <c r="G5" s="40">
         <v>6.3</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="43">
+        <v>5.6504815716081698</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>76</v>
       </c>
@@ -1017,7 +1036,7 @@
       <c r="F6" s="37"/>
       <c r="G6" s="40"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>12</v>
       </c>
@@ -1039,8 +1058,11 @@
       <c r="G7" s="41">
         <v>13.4</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="44">
+        <v>11.990552717185041</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>9</v>
       </c>
@@ -1062,8 +1084,11 @@
       <c r="G8" s="41">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="44">
+        <v>0.36686386493060885</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>15</v>
       </c>
@@ -1077,8 +1102,9 @@
       <c r="E9" s="38"/>
       <c r="F9" s="38"/>
       <c r="G9" s="41"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="44"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>18</v>
       </c>
@@ -1100,8 +1126,11 @@
       <c r="G10" s="41">
         <v>5.3</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="44">
+        <v>4.7585078053197183</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>21</v>
       </c>
@@ -1123,8 +1152,11 @@
       <c r="G11" s="41">
         <v>6.9</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="44">
+        <v>6.2147211180387529</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>24</v>
       </c>
@@ -1138,8 +1170,9 @@
       <c r="E12" s="38"/>
       <c r="F12" s="38"/>
       <c r="G12" s="41"/>
-    </row>
-    <row r="13" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H12" s="44"/>
+    </row>
+    <row r="13" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>27</v>
       </c>
@@ -1161,8 +1194,11 @@
       <c r="G13" s="41">
         <v>9.1</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H13" s="44">
+        <v>6.6299725226642234</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
         <v>30</v>
       </c>
@@ -1184,8 +1220,11 @@
       <c r="G14" s="41">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H14" s="44">
+        <v>1.0045350275012754</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
         <v>33</v>
       </c>
@@ -1207,8 +1246,11 @@
       <c r="G15" s="41">
         <v>15.2</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H15" s="44">
+        <v>15.32109744080277</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
         <v>36</v>
       </c>
@@ -1230,8 +1272,11 @@
       <c r="G16" s="41">
         <v>12.7</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H16" s="44">
+        <v>11.932654937916501</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
         <v>39</v>
       </c>
@@ -1253,8 +1298,11 @@
       <c r="G17" s="41">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H17" s="44">
+        <v>4.4024960942722968</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>42</v>
       </c>
@@ -1276,8 +1324,11 @@
       <c r="G18" s="41">
         <v>13</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H18" s="44">
+        <v>13.275841712798133</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>45</v>
       </c>
@@ -1299,8 +1350,11 @@
       <c r="G19" s="41">
         <v>7.8</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H19" s="44">
+        <v>5.5953228746387378</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>48</v>
       </c>
@@ -1322,8 +1376,11 @@
       <c r="G20" s="41">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H20" s="44">
+        <v>5.7561942305949083</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>51</v>
       </c>
@@ -1345,8 +1402,11 @@
       <c r="G21" s="41">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H21" s="44">
+        <v>0.91260128840317045</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>78</v>
       </c>
@@ -1360,8 +1420,9 @@
       <c r="E22" s="38"/>
       <c r="F22" s="38"/>
       <c r="G22" s="41"/>
-    </row>
-    <row r="23" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H22" s="44"/>
+    </row>
+    <row r="23" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
         <v>80</v>
       </c>
@@ -1383,8 +1444,11 @@
       <c r="G23" s="41">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H23" s="44">
+        <v>0.12558892880771302</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
         <v>81</v>
       </c>
@@ -1406,8 +1470,11 @@
       <c r="G24" s="41">
         <v>7.4</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H24" s="44">
+        <v>6.813728136595028</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
         <v>82</v>
       </c>
@@ -1429,8 +1496,11 @@
       <c r="G25" s="41">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="44">
+        <v>7.4835121062312364</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
         <v>84</v>
       </c>
@@ -1444,8 +1514,9 @@
       <c r="E26" s="38"/>
       <c r="F26" s="38"/>
       <c r="G26" s="41"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" s="44"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="31" t="s">
         <v>87</v>
       </c>
@@ -1467,8 +1538,11 @@
       <c r="G27" s="41">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27" s="44">
+        <v>1.0698262411858328</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="31" t="s">
         <v>54</v>
       </c>
@@ -1490,8 +1564,11 @@
       <c r="G28" s="41">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28" s="44">
+        <v>2.525977374670846</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="s">
         <v>56</v>
       </c>
@@ -1513,8 +1590,11 @@
       <c r="G29" s="41">
         <v>7.4</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" s="44">
+        <v>6.9014261042903025</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
         <v>58</v>
       </c>
@@ -1536,8 +1616,11 @@
       <c r="G30" s="41">
         <v>9.1</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30" s="44">
+        <v>7.9091356334900151</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
         <v>60</v>
       </c>
@@ -1559,8 +1642,11 @@
       <c r="G31" s="41">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31" s="44">
+        <v>3.3800067710254136</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="30" t="s">
         <v>62</v>
       </c>
@@ -1574,8 +1660,9 @@
       <c r="E32" s="38"/>
       <c r="F32" s="38"/>
       <c r="G32" s="41"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32" s="44"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="33" t="s">
         <v>64</v>
       </c>
@@ -1597,8 +1684,11 @@
       <c r="G33" s="41">
         <v>6.4</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33" s="44">
+        <v>4.7357406632935053</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="33" t="s">
         <v>66</v>
       </c>
@@ -1620,8 +1710,11 @@
       <c r="G34" s="41">
         <v>6.2</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34" s="44">
+        <v>4.7664658340238164</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="33" t="s">
         <v>68</v>
       </c>
@@ -1643,8 +1736,11 @@
       <c r="G35" s="41">
         <v>5.4</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35" s="44">
+        <v>5.4209310439574798</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="33" t="s">
         <v>70</v>
       </c>
@@ -1666,8 +1762,11 @@
       <c r="G36" s="41">
         <v>6.6</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H36" s="44">
+        <v>6.4917222807546029</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="34" t="s">
         <v>72</v>
       </c>
@@ -1689,8 +1788,11 @@
       <c r="G37" s="42">
         <v>7.2</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37" s="45">
+        <v>6.4231110817165149</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D38" s="18"/>
       <c r="E38" s="18"/>
       <c r="F38" s="18"/>

</xml_diff>